<commit_message>
Update with Manuel's remarks of concept paper.
</commit_message>
<xml_diff>
--- a/Dokumentation/MZ Liste Sensoren Aktoren.xlsx
+++ b/Dokumentation/MZ Liste Sensoren Aktoren.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Manuel\Nextcloud\Unterlagen\Studium\OTH AMBERG\IT und Automation Master\Semester 1\Semantic Web Technologien\Projekt\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Stefan Ries\Documents\Nextcloud\Studium_Master\Semester 1\Semantic Web\Projekt\GIT\opcua_netzwerk\Dokumentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{541C5149-0100-4452-92A1-65DBEA0FFCA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BDA3FBA-367B-4D55-B09C-735D3EAC0D3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2880" windowWidth="22654" windowHeight="12120" xr2:uid="{F4D0CA59-1170-47E4-83CC-A134CDEF6B7C}"/>
+    <workbookView xWindow="-21615" yWindow="900" windowWidth="14400" windowHeight="10755" xr2:uid="{F4D0CA59-1170-47E4-83CC-A134CDEF6B7C}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="74">
   <si>
     <t>Sensor</t>
   </si>
@@ -245,13 +245,19 @@
     <t>Luftqualitätssensor</t>
   </si>
   <si>
-    <t>MQ-5 ???</t>
-  </si>
-  <si>
     <t>Gas/CO2/…</t>
   </si>
   <si>
     <t>???</t>
+  </si>
+  <si>
+    <t>MQ-135</t>
+  </si>
+  <si>
+    <t>0-5V Analog</t>
+  </si>
+  <si>
+    <t>https://www.olimex.com/Products/Components/Sensors/Gas/SNS-MQ135/resources/SNS-MQ135.pdf</t>
   </si>
 </sst>
 </file>
@@ -275,7 +281,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -285,12 +291,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -311,8 +311,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -630,21 +630,21 @@
   <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="137" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:A15"/>
+      <selection activeCell="A6" sqref="A6:XFD6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.84375" customWidth="1"/>
-    <col min="2" max="2" width="19.3046875" customWidth="1"/>
-    <col min="3" max="3" width="5.15234375" customWidth="1"/>
-    <col min="5" max="5" width="18.07421875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21.15234375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.23046875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="109.23046875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.85546875" customWidth="1"/>
+    <col min="2" max="2" width="19.28515625" customWidth="1"/>
+    <col min="3" max="3" width="5.140625" customWidth="1"/>
+    <col min="5" max="5" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="109.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -670,7 +670,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -693,7 +693,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>10</v>
       </c>
@@ -719,7 +719,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>18</v>
       </c>
@@ -745,7 +745,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>27</v>
       </c>
@@ -771,30 +771,33 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>68</v>
       </c>
       <c r="B6" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="C6" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="D6" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="D6" s="4" t="s">
-        <v>71</v>
-      </c>
       <c r="E6" s="4" t="s">
-        <v>71</v>
+        <v>34</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="G6" s="4" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="H6" s="4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>33</v>
       </c>
@@ -818,7 +821,7 @@
       </c>
       <c r="H8" s="2"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>38</v>
       </c>
@@ -841,7 +844,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>37</v>
       </c>
@@ -864,7 +867,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>42</v>
       </c>
@@ -890,7 +893,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>42</v>
       </c>
@@ -916,7 +919,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>54</v>
       </c>
@@ -942,7 +945,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>63</v>
       </c>
@@ -968,7 +971,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>64</v>
       </c>

</xml_diff>